<commit_message>
fix: quản lý chấm công, xuất file báo cáo giai đoạn 2
</commit_message>
<xml_diff>
--- a/src/main/resources/excel-template/export-attendance-month-template.xlsx
+++ b/src/main/resources/excel-template/export-attendance-month-template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>BẢNG THỐNG KÊ CHẤM CÔNG</t>
   </si>
@@ -59,12 +59,30 @@
     <t>Tên nhân viên</t>
   </si>
   <si>
+    <t>Hệ số công</t>
+  </si>
+  <si>
+    <t>Tổng số giờ</t>
+  </si>
+  <si>
+    <t>Tổng phút phạt</t>
+  </si>
+  <si>
+    <t>Số giờ tăng ca</t>
+  </si>
+  <si>
+    <t>Số ngày nghỉ phép</t>
+  </si>
+  <si>
     <t>HRM</t>
   </si>
   <si>
     <t>&lt;jx:forEach items="${posLst}" var="item"&gt;</t>
   </si>
   <si>
+    <t>&lt;jx:forEach items="${item.checkInExportExcelResponse}" var="itemCheckIn"&gt;</t>
+  </si>
+  <si>
     <t>${item.index}</t>
   </si>
   <si>
@@ -77,154 +95,34 @@
     <t>Vào</t>
   </si>
   <si>
-    <t>${item.checkIn1}</t>
-  </si>
-  <si>
-    <t>${item.checkIn2}</t>
-  </si>
-  <si>
-    <t>${item.checkIn3}</t>
-  </si>
-  <si>
-    <t>off</t>
-  </si>
-  <si>
-    <t>${item.checkIn4}</t>
-  </si>
-  <si>
-    <t>${item.checkIn5}</t>
-  </si>
-  <si>
-    <t>${item.checkIn6}</t>
-  </si>
-  <si>
-    <t>${item.checkIn7}</t>
-  </si>
-  <si>
-    <t>${item.checkIn8}</t>
-  </si>
-  <si>
-    <t>${item.checkIn9}</t>
-  </si>
-  <si>
-    <t>${item.checkIn10}</t>
-  </si>
-  <si>
-    <t>${item.checkIn11}</t>
-  </si>
-  <si>
-    <t>${item.checkIn12}</t>
-  </si>
-  <si>
-    <t>${item.checkIn13}</t>
-  </si>
-  <si>
-    <t>${item.checkIn14}</t>
-  </si>
-  <si>
-    <t>${item.checkIn15}</t>
-  </si>
-  <si>
-    <t>${item.checkIn16}</t>
-  </si>
-  <si>
-    <t>${item.checkIn17}</t>
-  </si>
-  <si>
-    <t>${item.checkIn18}</t>
-  </si>
-  <si>
-    <t>${item.checkIn19}</t>
-  </si>
-  <si>
-    <t>${item.checkIn20}</t>
-  </si>
-  <si>
-    <t>${item.checkIn21}</t>
-  </si>
-  <si>
-    <t>${item.checkIn22}</t>
-  </si>
-  <si>
-    <t>${item.checkIn23}</t>
+    <t>&lt;jx:cell value="${itemCheckIn.checkIn}" row="${item.index+6}" col="${itemCheckIn.day+3}"/&gt;</t>
+  </si>
+  <si>
+    <t>${item.workingPoint}</t>
+  </si>
+  <si>
+    <t>${item.workingTime}</t>
+  </si>
+  <si>
+    <t>${item.totalPenalty}</t>
+  </si>
+  <si>
+    <t>${item.totalTimeOt}</t>
+  </si>
+  <si>
+    <t>${item.totalTimeLeave}</t>
+  </si>
+  <si>
+    <t>&lt;/jx:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${item.checkOutExportExcelResponse}" var="itemIndexOut"&gt;</t>
   </si>
   <si>
     <t>Ra</t>
   </si>
   <si>
-    <t>${item.checkOut1}</t>
-  </si>
-  <si>
-    <t>${item.checkOut2}</t>
-  </si>
-  <si>
-    <t>${item.checkOut3}</t>
-  </si>
-  <si>
-    <t>${item.checkOut4}</t>
-  </si>
-  <si>
-    <t>${item.checkOut5}</t>
-  </si>
-  <si>
-    <t>${item.checkOut6}</t>
-  </si>
-  <si>
-    <t>${item.checkOut7}</t>
-  </si>
-  <si>
-    <t>${item.checkOut8}</t>
-  </si>
-  <si>
-    <t>${item.checkOut9}</t>
-  </si>
-  <si>
-    <t>${item.checkOut10}</t>
-  </si>
-  <si>
-    <t>${item.checkOut11}</t>
-  </si>
-  <si>
-    <t>${item.checkOut12}</t>
-  </si>
-  <si>
-    <t>${item.checkOut13}</t>
-  </si>
-  <si>
-    <t>${item.checkOut14}</t>
-  </si>
-  <si>
-    <t>${item.checkOut15}</t>
-  </si>
-  <si>
-    <t>${item.checkOut16}</t>
-  </si>
-  <si>
-    <t>${item.checkOut17}</t>
-  </si>
-  <si>
-    <t>${item.checkOut18}</t>
-  </si>
-  <si>
-    <t>${item.checkOut19}</t>
-  </si>
-  <si>
-    <t>${item.checkOut20}</t>
-  </si>
-  <si>
-    <t>${item.checkOut21}</t>
-  </si>
-  <si>
-    <t>${item.checkOut22}</t>
-  </si>
-  <si>
-    <t>${item.checkOut23}</t>
-  </si>
-  <si>
-    <t>&lt;/jx:forEach&gt;</t>
-  </si>
-  <si>
-    <t>Ghi chú:</t>
+    <t>&lt;jx:cell value="${itemCheckOut.checkOut}" row="${item.index+7}" col="${itemCheckOut.day+3}"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -271,12 +169,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -287,6 +179,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -633,11 +533,24 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -678,6 +591,17 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -815,7 +739,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -827,34 +751,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -939,7 +863,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -961,74 +885,89 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1373,24 +1312,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AJ15"/>
+  <dimension ref="A1:AN24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10:AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6.83333333333333" customWidth="1"/>
     <col min="2" max="2" width="18.5555555555556" customWidth="1"/>
-    <col min="3" max="3" width="18.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="15.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="11.4444444444444" customWidth="1"/>
     <col min="5" max="5" width="10.3333333333333" customWidth="1"/>
     <col min="6" max="35" width="4.77777777777778" customWidth="1"/>
+    <col min="36" max="36" width="14.6666666666667" customWidth="1"/>
+    <col min="37" max="37" width="12.6666666666667" customWidth="1"/>
+    <col min="38" max="38" width="17.1111111111111" customWidth="1"/>
+    <col min="39" max="39" width="13.5555555555556" customWidth="1"/>
+    <col min="40" max="40" width="18.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" spans="1:35">
@@ -1460,7 +1404,7 @@
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="14" customHeight="1" spans="1:36">
+    <row r="5" s="1" customFormat="1" ht="14" customHeight="1" spans="1:40">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -1595,9 +1539,23 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AJ5" s="29"/>
+      <c r="AJ5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL5" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM5" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN5" s="35" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" s="2" customFormat="1" ht="12" customHeight="1" spans="1:36">
+    <row r="6" s="2" customFormat="1" ht="12" customHeight="1" spans="1:40">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1726,356 +1684,832 @@
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AJ6" s="30"/>
+      <c r="AJ6" s="35"/>
+      <c r="AK6" s="35"/>
+      <c r="AL6" s="35"/>
+      <c r="AM6" s="35"/>
+      <c r="AN6" s="35"/>
     </row>
-    <row r="7" s="2" customFormat="1" ht="19" customHeight="1" spans="1:36">
+    <row r="7" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
       <c r="A7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="18"/>
-      <c r="AH7" s="18"/>
-      <c r="AI7" s="31"/>
-      <c r="AJ7" s="30"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="17"/>
+      <c r="AG7" s="17"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="17"/>
+      <c r="AJ7" s="17"/>
+      <c r="AK7" s="17"/>
+      <c r="AL7" s="17"/>
+      <c r="AM7" s="17"/>
+      <c r="AN7" s="17"/>
     </row>
-    <row r="8" s="2" customFormat="1" ht="19" customHeight="1" spans="1:36">
-      <c r="A8" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
+    <row r="8" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="E8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
       <c r="V8" s="21"/>
       <c r="W8" s="21"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
       <c r="AC8" s="21"/>
       <c r="AD8" s="21"/>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="20"/>
-      <c r="AG8" s="20"/>
-      <c r="AH8" s="20"/>
-      <c r="AI8" s="32"/>
-      <c r="AJ8" s="30"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="21"/>
+      <c r="AH8" s="21"/>
+      <c r="AI8" s="36"/>
+      <c r="AJ8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK8" s="19"/>
+      <c r="AL8" s="19"/>
+      <c r="AM8" s="19"/>
+      <c r="AN8" s="37"/>
     </row>
-    <row r="9" s="2" customFormat="1" ht="19" customHeight="1" spans="1:36">
+    <row r="9" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
       <c r="A9" s="22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="D9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="E9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="25"/>
+      <c r="AJ9" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="24" t="s">
+      <c r="AK9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q9" s="24" t="s">
+      <c r="AL9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="24" t="s">
+      <c r="AM9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="AN9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="24" t="s">
+    </row>
+    <row r="10" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="U9" s="24" t="s">
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="30"/>
+      <c r="AI10" s="38"/>
+      <c r="AJ10" s="28"/>
+      <c r="AK10" s="28"/>
+      <c r="AL10" s="28"/>
+      <c r="AM10" s="28"/>
+      <c r="AN10" s="28"/>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="V9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="W9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="X9" s="24" t="s">
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="30"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="30"/>
+      <c r="AI11" s="38"/>
+      <c r="AJ11" s="28"/>
+      <c r="AK11" s="28"/>
+      <c r="AL11" s="28"/>
+      <c r="AM11" s="28"/>
+      <c r="AN11" s="28"/>
+    </row>
+    <row r="12" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="Y9" s="24" t="s">
+      <c r="E12" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="Z9" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA9" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE9" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF9" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH9" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI9" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ9" s="30"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="25"/>
+      <c r="AF12" s="25"/>
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="25"/>
+      <c r="AI12" s="25"/>
+      <c r="AJ12" s="28"/>
+      <c r="AK12" s="28"/>
+      <c r="AL12" s="28"/>
+      <c r="AM12" s="28"/>
+      <c r="AN12" s="28"/>
     </row>
-    <row r="10" customFormat="1" ht="17" customHeight="1" spans="1:36">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="M10" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q10" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="T10" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="U10" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="V10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="W10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="X10" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y10" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z10" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB10" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE10" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF10" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH10" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI10" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ10" s="10"/>
+    <row r="13" customFormat="1" ht="17" customHeight="1" spans="1:40">
+      <c r="A13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32"/>
+      <c r="AA13" s="32"/>
+      <c r="AB13" s="32"/>
+      <c r="AC13" s="32"/>
+      <c r="AD13" s="32"/>
+      <c r="AE13" s="32"/>
+      <c r="AF13" s="32"/>
+      <c r="AG13" s="32"/>
+      <c r="AH13" s="32"/>
+      <c r="AI13" s="33"/>
+      <c r="AJ13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK13" s="32"/>
+      <c r="AL13" s="32"/>
+      <c r="AM13" s="32"/>
+      <c r="AN13" s="33"/>
     </row>
-    <row r="11" ht="17" customHeight="1" spans="1:36">
-      <c r="A11" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="28"/>
-      <c r="W11" s="28"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="28"/>
-      <c r="AD11" s="28"/>
-      <c r="AE11" s="27"/>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="27"/>
-      <c r="AI11" s="33"/>
-      <c r="AJ11" s="10"/>
+    <row r="14" customFormat="1" ht="17" customHeight="1" spans="1:40">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="7"/>
+      <c r="AN14" s="7"/>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>64</v>
-      </c>
+    <row r="15" customFormat="1" ht="17" customHeight="1" spans="1:40">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+      <c r="AN15" s="7"/>
+    </row>
+    <row r="16" ht="17" customHeight="1" spans="1:40">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+      <c r="AN16" s="7"/>
+    </row>
+    <row r="17" ht="17" customHeight="1" spans="1:40">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="7"/>
+      <c r="AK17" s="7"/>
+      <c r="AL17" s="7"/>
+      <c r="AM17" s="7"/>
+      <c r="AN17" s="7"/>
+    </row>
+    <row r="18" spans="1:40">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="7"/>
+      <c r="AJ18" s="7"/>
+      <c r="AK18" s="7"/>
+      <c r="AL18" s="7"/>
+      <c r="AM18" s="7"/>
+      <c r="AN18" s="7"/>
+    </row>
+    <row r="19" spans="1:40">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="7"/>
+      <c r="AL19" s="7"/>
+      <c r="AM19" s="7"/>
+      <c r="AN19" s="7"/>
+    </row>
+    <row r="20" spans="1:40">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="7"/>
+      <c r="AL20" s="7"/>
+      <c r="AM20" s="7"/>
+      <c r="AN20" s="7"/>
+    </row>
+    <row r="21" spans="1:40">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7"/>
+      <c r="AL21" s="7"/>
+      <c r="AM21" s="7"/>
+      <c r="AN21" s="7"/>
+    </row>
+    <row r="22" spans="1:40">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+      <c r="AE22" s="7"/>
+      <c r="AF22" s="7"/>
+      <c r="AG22" s="7"/>
+      <c r="AH22" s="7"/>
+      <c r="AI22" s="7"/>
+      <c r="AJ22" s="7"/>
+      <c r="AK22" s="7"/>
+      <c r="AL22" s="7"/>
+      <c r="AM22" s="7"/>
+      <c r="AN22" s="7"/>
+    </row>
+    <row r="23" spans="1:40">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7"/>
+      <c r="AK23" s="7"/>
+      <c r="AL23" s="7"/>
+      <c r="AM23" s="7"/>
+      <c r="AN23" s="7"/>
+    </row>
+    <row r="24" spans="1:40">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="7"/>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="7"/>
+      <c r="AJ24" s="7"/>
+      <c r="AK24" s="7"/>
+      <c r="AL24" s="7"/>
+      <c r="AM24" s="7"/>
+      <c r="AN24" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="18">
     <mergeCell ref="A1:AI1"/>
-    <mergeCell ref="A8:AI8"/>
-    <mergeCell ref="A11:AI11"/>
+    <mergeCell ref="A7:AN7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:AI8"/>
+    <mergeCell ref="AJ8:AN8"/>
+    <mergeCell ref="E10:AI10"/>
+    <mergeCell ref="E11:AI11"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E13:AI13"/>
+    <mergeCell ref="AJ13:AN13"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A9:A10"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="AJ5:AJ6"/>
+    <mergeCell ref="AK5:AK6"/>
+    <mergeCell ref="AL5:AL6"/>
+    <mergeCell ref="AM5:AM6"/>
+    <mergeCell ref="AN5:AN6"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:AI7 E9:AI10">
+  <conditionalFormatting sqref="E5:AI6 E9:AI9 E12:AI12 D10:D11">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>IF(#REF!="Sun",1,0)</formula>
     </cfRule>
@@ -2083,7 +2517,7 @@
       <formula>IF(#REF!="Sun",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6:AI7 E9:AI10">
+  <conditionalFormatting sqref="E6:AI6 E9:AI9 D10:D11 E12:AI12">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF($E$6="CN",1,0)</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix: quản lý chấm công, xuất file báo cáo giai đoạn 3
</commit_message>
<xml_diff>
--- a/src/main/resources/excel-template/export-attendance-month-template.xlsx
+++ b/src/main/resources/excel-template/export-attendance-month-template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>BẢNG THỐNG KÊ CHẤM CÔNG</t>
   </si>
@@ -80,7 +80,10 @@
     <t>&lt;jx:forEach items="${posLst}" var="item"&gt;</t>
   </si>
   <si>
-    <t>&lt;jx:forEach items="${item.checkInExportExcelResponse}" var="itemCheckIn"&gt;</t>
+    <t>&lt;jx:forEach items="${item.checkIn}" var="checkInResponse"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${checkInResponse.checkIn}" var="checkInValue"&gt;</t>
   </si>
   <si>
     <t>${item.index}</t>
@@ -95,9 +98,6 @@
     <t>Vào</t>
   </si>
   <si>
-    <t>&lt;jx:cell value="${itemCheckIn.checkIn}" row="${item.index+6}" col="${itemCheckIn.day+3}"/&gt;</t>
-  </si>
-  <si>
     <t>${item.workingPoint}</t>
   </si>
   <si>
@@ -113,16 +113,31 @@
     <t>${item.totalTimeLeave}</t>
   </si>
   <si>
+    <t>&lt;jx:cell value="${checkInValue}" row="${rowNumber}" col="${colNumber}"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:increment var="colNumber" count="1"/&gt;</t>
+  </si>
+  <si>
     <t>&lt;/jx:forEach&gt;</t>
   </si>
   <si>
-    <t>&lt;jx:forEach items="${item.checkOutExportExcelResponse}" var="itemIndexOut"&gt;</t>
+    <t>&lt;jx:increment var="rowNumber" count="1"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:assign var="colNumber" value="4"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;jx:forEach items="${item.checkOut}" var="checkOutResponse"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;jx:forEach items="${checkOutResponse.checkOut}" var="checkOutValue"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:cell value="${checkOutValue}" row="${rowNumber}" col="${colNumber}"/&gt;</t>
   </si>
   <si>
     <t>Ra</t>
-  </si>
-  <si>
-    <t>&lt;jx:cell value="${itemCheckOut.checkOut}" row="${item.index+7}" col="${itemCheckOut.day+3}"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -137,7 +152,7 @@
     <numFmt numFmtId="178" formatCode="dd"/>
     <numFmt numFmtId="179" formatCode="&quot;T&quot;General"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,12 +187,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -533,7 +542,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -573,17 +582,30 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color auto="1"/>
-      </top>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -597,10 +619,10 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
-      </right>
-      <top/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -612,9 +634,25 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
-      </bottom>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -733,137 +771,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -906,17 +944,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -933,41 +962,38 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1312,21 +1338,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AN24"/>
+  <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10:AI10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6.83333333333333" customWidth="1"/>
     <col min="2" max="2" width="18.5555555555556" customWidth="1"/>
-    <col min="3" max="3" width="15.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="21.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="11.4444444444444" customWidth="1"/>
     <col min="5" max="5" width="10.3333333333333" customWidth="1"/>
     <col min="6" max="35" width="4.77777777777778" customWidth="1"/>
@@ -1539,19 +1561,19 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AJ5" s="35" t="s">
+      <c r="AJ5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="AK5" s="35" t="s">
+      <c r="AK5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AL5" s="35" t="s">
+      <c r="AL5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AM5" s="35" t="s">
+      <c r="AM5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="AN5" s="35" t="s">
+      <c r="AN5" s="29" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1684,11 +1706,11 @@
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="35"/>
-      <c r="AL6" s="35"/>
-      <c r="AM6" s="35"/>
-      <c r="AN6" s="35"/>
+      <c r="AJ6" s="29"/>
+      <c r="AK6" s="29"/>
+      <c r="AL6" s="29"/>
+      <c r="AM6" s="29"/>
+      <c r="AN6" s="29"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
       <c r="A7" s="17" t="s">
@@ -1738,768 +1760,1258 @@
       <c r="A8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="20"/>
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="20"/>
+      <c r="AM8" s="20"/>
+      <c r="AN8" s="20"/>
+    </row>
+    <row r="9" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
-      <c r="AE8" s="21"/>
-      <c r="AF8" s="21"/>
-      <c r="AG8" s="21"/>
-      <c r="AH8" s="21"/>
-      <c r="AI8" s="36"/>
-      <c r="AJ8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK8" s="19"/>
-      <c r="AL8" s="19"/>
-      <c r="AM8" s="19"/>
-      <c r="AN8" s="37"/>
-    </row>
-    <row r="9" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
-      <c r="A9" s="22" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="22"/>
+      <c r="AI9" s="30"/>
+      <c r="AJ9" s="31"/>
+      <c r="AK9" s="31"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="32"/>
+      <c r="AN9" s="32"/>
+    </row>
+    <row r="10" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="22"/>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="31"/>
+      <c r="AK10" s="31"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="32"/>
+      <c r="AN10" s="32"/>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="C11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="D11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="25"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="25"/>
-      <c r="AF9" s="25"/>
-      <c r="AG9" s="25"/>
-      <c r="AH9" s="25"/>
-      <c r="AI9" s="25"/>
-      <c r="AJ9" s="23" t="s">
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="22"/>
+      <c r="AG11" s="22"/>
+      <c r="AH11" s="22"/>
+      <c r="AI11" s="30"/>
+      <c r="AJ11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AK9" s="23" t="s">
+      <c r="AK11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AL9" s="23" t="s">
+      <c r="AL11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="AM9" s="23" t="s">
+      <c r="AM11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="AN9" s="23" t="s">
+      <c r="AN11" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30" t="s">
+    <row r="12" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A12" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
-      <c r="AB10" s="30"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="30"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30"/>
-      <c r="AG10" s="30"/>
-      <c r="AH10" s="30"/>
-      <c r="AI10" s="38"/>
-      <c r="AJ10" s="28"/>
-      <c r="AK10" s="28"/>
-      <c r="AL10" s="28"/>
-      <c r="AM10" s="28"/>
-      <c r="AN10" s="28"/>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="23"/>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="22"/>
+      <c r="AH12" s="22"/>
+      <c r="AI12" s="30"/>
+      <c r="AJ12" s="33"/>
+      <c r="AK12" s="33"/>
+      <c r="AL12" s="25"/>
+      <c r="AM12" s="34"/>
+      <c r="AN12" s="34"/>
+    </row>
+    <row r="13" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="30"/>
-      <c r="AA11" s="30"/>
-      <c r="AB11" s="30"/>
-      <c r="AC11" s="30"/>
-      <c r="AD11" s="30"/>
-      <c r="AE11" s="30"/>
-      <c r="AF11" s="30"/>
-      <c r="AG11" s="30"/>
-      <c r="AH11" s="30"/>
-      <c r="AI11" s="38"/>
-      <c r="AJ11" s="28"/>
-      <c r="AK11" s="28"/>
-      <c r="AL11" s="28"/>
-      <c r="AM11" s="28"/>
-      <c r="AN11" s="28"/>
-    </row>
-    <row r="12" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="24" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="22"/>
+      <c r="AA13" s="22"/>
+      <c r="AB13" s="22"/>
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="22"/>
+      <c r="AF13" s="22"/>
+      <c r="AG13" s="22"/>
+      <c r="AH13" s="22"/>
+      <c r="AI13" s="30"/>
+      <c r="AJ13" s="33"/>
+      <c r="AK13" s="33"/>
+      <c r="AL13" s="25"/>
+      <c r="AM13" s="34"/>
+      <c r="AN13" s="34"/>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A14" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="22"/>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="23"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="22"/>
+      <c r="AF14" s="22"/>
+      <c r="AG14" s="22"/>
+      <c r="AH14" s="22"/>
+      <c r="AI14" s="30"/>
+      <c r="AJ14" s="33"/>
+      <c r="AK14" s="33"/>
+      <c r="AL14" s="25"/>
+      <c r="AM14" s="34"/>
+      <c r="AN14" s="34"/>
+    </row>
+    <row r="15" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="22"/>
+      <c r="AA15" s="22"/>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="23"/>
+      <c r="AD15" s="23"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="22"/>
+      <c r="AG15" s="22"/>
+      <c r="AH15" s="22"/>
+      <c r="AI15" s="30"/>
+      <c r="AJ15" s="33"/>
+      <c r="AK15" s="33"/>
+      <c r="AL15" s="25"/>
+      <c r="AM15" s="34"/>
+      <c r="AN15" s="34"/>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A16" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="26"/>
-      <c r="AD12" s="26"/>
-      <c r="AE12" s="25"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="25"/>
-      <c r="AI12" s="25"/>
-      <c r="AJ12" s="28"/>
-      <c r="AK12" s="28"/>
-      <c r="AL12" s="28"/>
-      <c r="AM12" s="28"/>
-      <c r="AN12" s="28"/>
-    </row>
-    <row r="13" customFormat="1" ht="17" customHeight="1" spans="1:40">
-      <c r="A13" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="32"/>
-      <c r="AC13" s="32"/>
-      <c r="AD13" s="32"/>
-      <c r="AE13" s="32"/>
-      <c r="AF13" s="32"/>
-      <c r="AG13" s="32"/>
-      <c r="AH13" s="32"/>
-      <c r="AI13" s="33"/>
-      <c r="AJ13" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK13" s="32"/>
-      <c r="AL13" s="32"/>
-      <c r="AM13" s="32"/>
-      <c r="AN13" s="33"/>
-    </row>
-    <row r="14" customFormat="1" ht="17" customHeight="1" spans="1:40">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
-      <c r="AE14" s="7"/>
-      <c r="AF14" s="7"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="7"/>
-      <c r="AK14" s="7"/>
-      <c r="AL14" s="7"/>
-      <c r="AM14" s="7"/>
-      <c r="AN14" s="7"/>
-    </row>
-    <row r="15" customFormat="1" ht="17" customHeight="1" spans="1:40">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="7"/>
-      <c r="AI15" s="7"/>
-      <c r="AJ15" s="7"/>
-      <c r="AK15" s="7"/>
-      <c r="AL15" s="7"/>
-      <c r="AM15" s="7"/>
-      <c r="AN15" s="7"/>
-    </row>
-    <row r="16" ht="17" customHeight="1" spans="1:40">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="7"/>
-      <c r="AE16" s="7"/>
-      <c r="AF16" s="7"/>
-      <c r="AG16" s="7"/>
-      <c r="AH16" s="7"/>
-      <c r="AI16" s="7"/>
-      <c r="AJ16" s="7"/>
-      <c r="AK16" s="7"/>
-      <c r="AL16" s="7"/>
-      <c r="AM16" s="7"/>
-      <c r="AN16" s="7"/>
-    </row>
-    <row r="17" ht="17" customHeight="1" spans="1:40">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
-      <c r="AF17" s="7"/>
-      <c r="AG17" s="7"/>
-      <c r="AH17" s="7"/>
-      <c r="AI17" s="7"/>
-      <c r="AJ17" s="7"/>
-      <c r="AK17" s="7"/>
-      <c r="AL17" s="7"/>
-      <c r="AM17" s="7"/>
-      <c r="AN17" s="7"/>
-    </row>
-    <row r="18" spans="1:40">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="7"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
-      <c r="AF18" s="7"/>
-      <c r="AG18" s="7"/>
-      <c r="AH18" s="7"/>
-      <c r="AI18" s="7"/>
-      <c r="AJ18" s="7"/>
-      <c r="AK18" s="7"/>
-      <c r="AL18" s="7"/>
-      <c r="AM18" s="7"/>
-      <c r="AN18" s="7"/>
-    </row>
-    <row r="19" spans="1:40">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
-      <c r="AC19" s="7"/>
-      <c r="AD19" s="7"/>
-      <c r="AE19" s="7"/>
-      <c r="AF19" s="7"/>
-      <c r="AG19" s="7"/>
-      <c r="AH19" s="7"/>
-      <c r="AI19" s="7"/>
-      <c r="AJ19" s="7"/>
-      <c r="AK19" s="7"/>
-      <c r="AL19" s="7"/>
-      <c r="AM19" s="7"/>
-      <c r="AN19" s="7"/>
-    </row>
-    <row r="20" spans="1:40">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="7"/>
-      <c r="AB20" s="7"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-      <c r="AE20" s="7"/>
-      <c r="AF20" s="7"/>
-      <c r="AG20" s="7"/>
-      <c r="AH20" s="7"/>
-      <c r="AI20" s="7"/>
-      <c r="AJ20" s="7"/>
-      <c r="AK20" s="7"/>
-      <c r="AL20" s="7"/>
-      <c r="AM20" s="7"/>
-      <c r="AN20" s="7"/>
-    </row>
-    <row r="21" spans="1:40">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-      <c r="AB21" s="7"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
-      <c r="AI21" s="7"/>
-      <c r="AJ21" s="7"/>
-      <c r="AK21" s="7"/>
-      <c r="AL21" s="7"/>
-      <c r="AM21" s="7"/>
-      <c r="AN21" s="7"/>
-    </row>
-    <row r="22" spans="1:40">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
-      <c r="AA22" s="7"/>
-      <c r="AB22" s="7"/>
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
-      <c r="AF22" s="7"/>
-      <c r="AG22" s="7"/>
-      <c r="AH22" s="7"/>
-      <c r="AI22" s="7"/>
-      <c r="AJ22" s="7"/>
-      <c r="AK22" s="7"/>
-      <c r="AL22" s="7"/>
-      <c r="AM22" s="7"/>
-      <c r="AN22" s="7"/>
-    </row>
-    <row r="23" spans="1:40">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="7"/>
-      <c r="AH23" s="7"/>
-      <c r="AI23" s="7"/>
-      <c r="AJ23" s="7"/>
-      <c r="AK23" s="7"/>
-      <c r="AL23" s="7"/>
-      <c r="AM23" s="7"/>
-      <c r="AN23" s="7"/>
-    </row>
-    <row r="24" spans="1:40">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
-      <c r="AJ24" s="7"/>
-      <c r="AK24" s="7"/>
-      <c r="AL24" s="7"/>
-      <c r="AM24" s="7"/>
-      <c r="AN24" s="7"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="23"/>
+      <c r="AD16" s="23"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="22"/>
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="22"/>
+      <c r="AI16" s="30"/>
+      <c r="AJ16" s="33"/>
+      <c r="AK16" s="33"/>
+      <c r="AL16" s="25"/>
+      <c r="AM16" s="34"/>
+      <c r="AN16" s="34"/>
+    </row>
+    <row r="17" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A17" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+      <c r="AH17" s="22"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="33"/>
+      <c r="AK17" s="33"/>
+      <c r="AL17" s="25"/>
+      <c r="AM17" s="34"/>
+      <c r="AN17" s="34"/>
+    </row>
+    <row r="18" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A18" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="23"/>
+      <c r="AD18" s="23"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+      <c r="AG18" s="22"/>
+      <c r="AH18" s="22"/>
+      <c r="AI18" s="30"/>
+      <c r="AJ18" s="33"/>
+      <c r="AK18" s="33"/>
+      <c r="AL18" s="25"/>
+      <c r="AM18" s="34"/>
+      <c r="AN18" s="34"/>
+    </row>
+    <row r="19" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A19" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22"/>
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
+      <c r="AG19" s="22"/>
+      <c r="AH19" s="22"/>
+      <c r="AI19" s="30"/>
+      <c r="AJ19" s="33"/>
+      <c r="AK19" s="33"/>
+      <c r="AL19" s="25"/>
+      <c r="AM19" s="34"/>
+      <c r="AN19" s="34"/>
+    </row>
+    <row r="20" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A20" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
+      <c r="AG20" s="22"/>
+      <c r="AH20" s="22"/>
+      <c r="AI20" s="22"/>
+      <c r="AJ20" s="27"/>
+      <c r="AK20" s="27"/>
+      <c r="AL20" s="27"/>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="27"/>
+    </row>
+    <row r="21" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A21" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="28"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="28"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="28"/>
+      <c r="AH21" s="28"/>
+      <c r="AI21" s="28"/>
+      <c r="AJ21" s="26"/>
+      <c r="AK21" s="26"/>
+      <c r="AL21" s="26"/>
+      <c r="AM21" s="26"/>
+      <c r="AN21" s="26"/>
+    </row>
+    <row r="22" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A22" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="28"/>
+      <c r="Y22" s="28"/>
+      <c r="Z22" s="28"/>
+      <c r="AA22" s="28"/>
+      <c r="AB22" s="28"/>
+      <c r="AC22" s="28"/>
+      <c r="AD22" s="28"/>
+      <c r="AE22" s="28"/>
+      <c r="AF22" s="28"/>
+      <c r="AG22" s="28"/>
+      <c r="AH22" s="28"/>
+      <c r="AI22" s="28"/>
+      <c r="AJ22" s="26"/>
+      <c r="AK22" s="26"/>
+      <c r="AL22" s="26"/>
+      <c r="AM22" s="26"/>
+      <c r="AN22" s="26"/>
+    </row>
+    <row r="23" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A23" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="28"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="28"/>
+      <c r="Z23" s="28"/>
+      <c r="AA23" s="28"/>
+      <c r="AB23" s="28"/>
+      <c r="AC23" s="28"/>
+      <c r="AD23" s="28"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="28"/>
+      <c r="AI23" s="28"/>
+      <c r="AJ23" s="26"/>
+      <c r="AK23" s="26"/>
+      <c r="AL23" s="26"/>
+      <c r="AM23" s="26"/>
+      <c r="AN23" s="26"/>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A24" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="28"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="28"/>
+      <c r="AD24" s="28"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="28"/>
+      <c r="AH24" s="28"/>
+      <c r="AI24" s="28"/>
+      <c r="AJ24" s="26"/>
+      <c r="AK24" s="26"/>
+      <c r="AL24" s="26"/>
+      <c r="AM24" s="26"/>
+      <c r="AN24" s="26"/>
+    </row>
+    <row r="25" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A25" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="28"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="28"/>
+      <c r="X25" s="28"/>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="28"/>
+      <c r="AA25" s="28"/>
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="28"/>
+      <c r="AD25" s="28"/>
+      <c r="AE25" s="28"/>
+      <c r="AF25" s="28"/>
+      <c r="AG25" s="28"/>
+      <c r="AH25" s="28"/>
+      <c r="AI25" s="28"/>
+      <c r="AJ25" s="26"/>
+      <c r="AK25" s="26"/>
+      <c r="AL25" s="26"/>
+      <c r="AM25" s="26"/>
+      <c r="AN25" s="26"/>
+    </row>
+    <row r="26" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="28"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="28"/>
+      <c r="X26" s="28"/>
+      <c r="Y26" s="28"/>
+      <c r="Z26" s="28"/>
+      <c r="AA26" s="28"/>
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="28"/>
+      <c r="AD26" s="28"/>
+      <c r="AE26" s="28"/>
+      <c r="AF26" s="28"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="28"/>
+      <c r="AI26" s="28"/>
+      <c r="AJ26" s="28"/>
+      <c r="AK26" s="28"/>
+      <c r="AL26" s="28"/>
+      <c r="AM26" s="28"/>
+      <c r="AN26" s="28"/>
+    </row>
+    <row r="27" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="7"/>
+      <c r="AD27" s="7"/>
+      <c r="AE27" s="7"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7"/>
+      <c r="AK27" s="7"/>
+      <c r="AL27" s="7"/>
+      <c r="AM27" s="7"/>
+      <c r="AN27" s="7"/>
+    </row>
+    <row r="28" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
+      <c r="AB28" s="7"/>
+      <c r="AC28" s="7"/>
+      <c r="AD28" s="7"/>
+      <c r="AE28" s="7"/>
+      <c r="AF28" s="7"/>
+      <c r="AG28" s="7"/>
+      <c r="AH28" s="7"/>
+      <c r="AI28" s="7"/>
+      <c r="AJ28" s="7"/>
+      <c r="AK28" s="7"/>
+      <c r="AL28" s="7"/>
+      <c r="AM28" s="7"/>
+      <c r="AN28" s="7"/>
+    </row>
+    <row r="29" s="2" customFormat="1" ht="19" customHeight="1" spans="1:40">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
+      <c r="AC29" s="7"/>
+      <c r="AD29" s="7"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="7"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="7"/>
+      <c r="AJ29" s="7"/>
+      <c r="AK29" s="7"/>
+      <c r="AL29" s="7"/>
+      <c r="AM29" s="7"/>
+      <c r="AN29" s="7"/>
+    </row>
+    <row r="30" customFormat="1" ht="17" customHeight="1" spans="1:40">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7"/>
+      <c r="AE30" s="7"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="7"/>
+      <c r="AH30" s="7"/>
+      <c r="AI30" s="7"/>
+      <c r="AJ30" s="7"/>
+      <c r="AK30" s="7"/>
+      <c r="AL30" s="7"/>
+      <c r="AM30" s="7"/>
+      <c r="AN30" s="7"/>
+    </row>
+    <row r="31" customFormat="1" ht="17" customHeight="1" spans="1:40">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7"/>
+      <c r="AL31" s="7"/>
+      <c r="AM31" s="7"/>
+      <c r="AN31" s="7"/>
+    </row>
+    <row r="32" customFormat="1" ht="17" customHeight="1" spans="1:40">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7"/>
+      <c r="AE32" s="7"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
+      <c r="AI32" s="7"/>
+      <c r="AJ32" s="7"/>
+      <c r="AK32" s="7"/>
+      <c r="AL32" s="7"/>
+      <c r="AM32" s="7"/>
+      <c r="AN32" s="7"/>
+    </row>
+    <row r="33" ht="17" customHeight="1" spans="1:40">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7"/>
+      <c r="AL33" s="7"/>
+      <c r="AM33" s="7"/>
+      <c r="AN33" s="7"/>
+    </row>
+    <row r="34" ht="17" customHeight="1" spans="1:40">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="7"/>
+      <c r="AJ34" s="7"/>
+      <c r="AK34" s="7"/>
+      <c r="AL34" s="7"/>
+      <c r="AM34" s="7"/>
+      <c r="AN34" s="7"/>
+    </row>
+    <row r="35" spans="1:40">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7"/>
+      <c r="AK35" s="7"/>
+      <c r="AL35" s="7"/>
+      <c r="AM35" s="7"/>
+      <c r="AN35" s="7"/>
+    </row>
+    <row r="36" spans="1:40">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="AJ36" s="7"/>
+      <c r="AK36" s="7"/>
+      <c r="AL36" s="7"/>
+      <c r="AM36" s="7"/>
+      <c r="AN36" s="7"/>
+    </row>
+    <row r="37" spans="1:40">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7"/>
+      <c r="AL37" s="7"/>
+      <c r="AM37" s="7"/>
+      <c r="AN37" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="10">
     <mergeCell ref="A1:AI1"/>
     <mergeCell ref="A7:AN7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:AI8"/>
-    <mergeCell ref="AJ8:AN8"/>
-    <mergeCell ref="E10:AI10"/>
-    <mergeCell ref="E11:AI11"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E13:AI13"/>
-    <mergeCell ref="AJ13:AN13"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -2509,7 +3021,7 @@
     <mergeCell ref="AM5:AM6"/>
     <mergeCell ref="AN5:AN6"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:AI6 E9:AI9 E12:AI12 D10:D11">
+  <conditionalFormatting sqref="E5:AI6 E11:AI25">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>IF(#REF!="Sun",1,0)</formula>
     </cfRule>
@@ -2517,7 +3029,7 @@
       <formula>IF(#REF!="Sun",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6:AI6 E9:AI9 D10:D11 E12:AI12">
+  <conditionalFormatting sqref="E6:AI6 E11:AI25">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF($E$6="CN",1,0)</formula>
     </cfRule>

</xml_diff>